<commit_message>
Doc: Casos de uso
</commit_message>
<xml_diff>
--- a/Tablas.xlsx
+++ b/Tablas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xoel\Desktop\A Carballeira\2DAM\PFC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151B9E4D-9991-4CD9-BC81-5379A33295AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DEF383-A980-42D9-9846-DADA6CA84947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{11D5D283-4BA0-45B7-AEE6-C6A22E61ED0D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{11D5D283-4BA0-45B7-AEE6-C6A22E61ED0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablas BD" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="112">
   <si>
     <t>PK</t>
   </si>
@@ -285,9 +285,6 @@
     <t>Actor</t>
   </si>
   <si>
-    <t>Usuario</t>
-  </si>
-  <si>
     <t>El usuario pulsa el botón "+" para añadir un libro. Introduce el título, autor o ISBN en el buscador y se muestran las posibles coincidencias. Al seleccionar un libro, este se añade a su biblioteca personal con los datos recuperados automáticamente desde la API (si están disponibles).</t>
   </si>
   <si>
@@ -301,6 +298,81 @@
   </si>
   <si>
     <t>El libro queda registrado en la biblioteca del usuario. A nivel interno, si el autor, género o editorial no existiera previamente en la base de datos, se crean automáticamente para mantener las relaciones correctas.</t>
+  </si>
+  <si>
+    <t>CASO DE USO 2: EDITAR UN LIBRO</t>
+  </si>
+  <si>
+    <t>El usuario accede a los detalles de un libro previamente añadido y modifica uno o varios campos: fechas de lectura, reseña personal, calificación, estado, etc.</t>
+  </si>
+  <si>
+    <t>Los cambios realizados por el usuario se guardan correctamente en la base de datos, actualizando el registro del libro.</t>
+  </si>
+  <si>
+    <t>El libro ya debe estar registrado en la biblioteca del usuario.</t>
+  </si>
+  <si>
+    <t>Añadir un libro.</t>
+  </si>
+  <si>
+    <t>Usuario.</t>
+  </si>
+  <si>
+    <t>Editar un libro.</t>
+  </si>
+  <si>
+    <t>CASO DE USO 3: ELIMINAR UN LIBRO</t>
+  </si>
+  <si>
+    <t>Eliminar un libro.</t>
+  </si>
+  <si>
+    <t>El usuario selecciona un libro de su biblioteca personal y lo elimina permanentemente.</t>
+  </si>
+  <si>
+    <t>El libro se elimina de la base de datos. Las relaciones con autores, géneros o editorial también se eliminan si ya no están vinculadas a otros libros.</t>
+  </si>
+  <si>
+    <t>CASO DE USO 4: BUSCAR LIBROS</t>
+  </si>
+  <si>
+    <t>Buscar libros.</t>
+  </si>
+  <si>
+    <t>Desde la vista principal (vista en la que se muestran los libros añadidos por el usuario a su biblioteca), el usuario introduce un término de búsqueda (título, autor o ISBN) en el buscador para localizar libros específicos.</t>
+  </si>
+  <si>
+    <t>Deben existir libros previamente añadidos por el usuario.</t>
+  </si>
+  <si>
+    <t>La vista principal se actualiza mostrando únicamente los libros que coinciden con el criterio de búsqueda.</t>
+  </si>
+  <si>
+    <t>CASO DE USO 5: FILTRAR LIBROS</t>
+  </si>
+  <si>
+    <t>Filtrar libros.</t>
+  </si>
+  <si>
+    <t>El usuario aplica uno o varios filtros desde la interfaz principal para visualizar solo los libros que cumplan ciertos criterios: género, serie, estado, calificación, etc.</t>
+  </si>
+  <si>
+    <t>La lista de libros mostrada se actualiza para reflejar solo aquellos que cumplen con los filtros aplicados.</t>
+  </si>
+  <si>
+    <t>CASO DE USO 6: VER ESTADÍSTICAS</t>
+  </si>
+  <si>
+    <t>Ver estadísticas.</t>
+  </si>
+  <si>
+    <t>El usuario accede a una sección de la aplicación que muestra datos estadísticos basados en los libros de su biblioteca.</t>
+  </si>
+  <si>
+    <t>Deben existir libros añadidos con información suficiente (estado de lectura, calificación, fechas, etc.).</t>
+  </si>
+  <si>
+    <t>Se muestra al usuario un resumen visual o textual de estadísticas como número total de libros, libros leídos, media de calificación, etc.</t>
   </si>
 </sst>
 </file>
@@ -683,24 +755,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -710,41 +812,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -753,7 +825,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="24">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -761,43 +836,67 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -861,6 +960,39 @@
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -880,7 +1012,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3580BE9-19D9-4226-A531-EAB7E1E7B707}" name="Tabla1" displayName="Tabla1" ref="B2:E21" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3580BE9-19D9-4226-A531-EAB7E1E7B707}" name="Tabla1" displayName="Tabla1" ref="B2:E21" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="B2:E21" xr:uid="{A3580BE9-19D9-4226-A531-EAB7E1E7B707}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -888,24 +1020,94 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{02BCE4A8-9E29-4081-86C4-CC2E1D82791E}" name="Fase" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{C8D57AC5-20ED-437C-8900-3789D4A8BC25}" name="Tiempo estimado" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{DAE254B1-C70D-458D-973F-5006E8EBEB8B}" name="Inicio" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{C0EA90E3-1365-4B0A-805E-83353688EC11}" name="Fin" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{02BCE4A8-9E29-4081-86C4-CC2E1D82791E}" name="Fase" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{C8D57AC5-20ED-437C-8900-3789D4A8BC25}" name="Tiempo estimado" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{DAE254B1-C70D-458D-973F-5006E8EBEB8B}" name="Inicio" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{C0EA90E3-1365-4B0A-805E-83353688EC11}" name="Fin" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{35D9FBFC-1314-4A7C-A358-B29E72364FB8}" name="Tabla5" displayName="Tabla5" ref="B3:C8" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{35D9FBFC-1314-4A7C-A358-B29E72364FB8}" name="Tabla5" displayName="Tabla5" ref="B3:C8" totalsRowShown="0" headerRowDxfId="17">
   <autoFilter ref="B3:C8" xr:uid="{35D9FBFC-1314-4A7C-A358-B29E72364FB8}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{B9465E2E-C568-499E-BA0C-90A7552A7662}" name="Campo" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{3CF3611C-CFF7-4246-930B-F666D8CA7927}" name="Descripción" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{B9465E2E-C568-499E-BA0C-90A7552A7662}" name="Campo" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{3CF3611C-CFF7-4246-930B-F666D8CA7927}" name="Descripción" dataDxfId="15"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4AAE1917-C13A-4CDF-B275-F08A045DAFE6}" name="Tabla53" displayName="Tabla53" ref="B11:C16" totalsRowShown="0" headerRowDxfId="14">
+  <autoFilter ref="B11:C16" xr:uid="{4AAE1917-C13A-4CDF-B275-F08A045DAFE6}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{746F11CB-73EF-48D0-A103-6082BFA4840D}" name="Campo" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{5A63AE89-EBA0-4B1C-A759-57B1454AD949}" name="Descripción" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C92D463C-1773-45B1-BE84-D28B2B4C0FD3}" name="Tabla534" displayName="Tabla534" ref="B19:C24" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="B19:C24" xr:uid="{C92D463C-1773-45B1-BE84-D28B2B4C0FD3}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{B0231060-EB1A-414C-9CB7-2B3555D1B5EB}" name="Campo" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{283AE2CC-2976-4B96-9CBB-8DA22B7E4BBC}" name="Descripción" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{28243E43-C480-424E-AE9B-4642FA5901BA}" name="Tabla5345" displayName="Tabla5345" ref="B27:C32" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="B27:C32" xr:uid="{28243E43-C480-424E-AE9B-4642FA5901BA}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{495E8330-EB37-43CF-AD89-2059C11F972B}" name="Campo" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{E698F615-40DE-4255-8FE4-E9BE3ED6621B}" name="Descripción" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BBED26D4-7CB2-43A3-8A0D-EFB57C8CBCAE}" name="Tabla53457" displayName="Tabla53457" ref="B35:C40" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="B35:C40" xr:uid="{BBED26D4-7CB2-43A3-8A0D-EFB57C8CBCAE}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{7B66B3BD-5CF1-4705-9F4D-0354B9C0BF7A}" name="Campo" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{2EA9C0F4-971D-400D-93DB-A3567A1FAF38}" name="Descripción" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1B74E673-8337-4E9D-AC1A-1CD7434921E6}" name="Tabla534578" displayName="Tabla534578" ref="B43:C48" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="B43:C48" xr:uid="{1B74E673-8337-4E9D-AC1A-1CD7434921E6}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{3F70A758-7B26-45A9-AA70-7C6ECE322353}" name="Campo" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{AFB2C923-0B4F-4BE0-ABBA-BD129C347F42}" name="Descripción" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1237,25 +1439,25 @@
   <sheetData>
     <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="32"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="42"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -1314,24 +1516,24 @@
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="28" t="s">
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28" t="s">
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1339,30 +1541,30 @@
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
     </row>
     <row r="6" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="25"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="31"/>
       <c r="E7" s="14"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
@@ -1391,18 +1593,18 @@
       <c r="B10" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="35"/>
+      <c r="D10" s="37"/>
       <c r="E10" s="12"/>
     </row>
     <row r="11" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="25"/>
+      <c r="C12" s="31"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
@@ -1430,10 +1632,10 @@
     </row>
     <row r="16" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="25"/>
+      <c r="C17" s="31"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
@@ -1461,10 +1663,10 @@
     </row>
     <row r="21" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="25"/>
+      <c r="C22" s="31"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
@@ -1475,10 +1677,10 @@
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="27"/>
+      <c r="C24" s="35"/>
     </row>
     <row r="25" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
@@ -1490,10 +1692,10 @@
     </row>
     <row r="26" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="25"/>
+      <c r="C27" s="31"/>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="9" t="s">
@@ -1504,10 +1706,10 @@
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="27"/>
+      <c r="C29" s="35"/>
     </row>
     <row r="30" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
@@ -1519,16 +1721,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="G4:G5"/>
@@ -1544,6 +1736,16 @@
     <mergeCell ref="R4:R5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1566,10 +1768,10 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="38"/>
+      <c r="C2" s="44"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
@@ -1637,8 +1839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48A83546-915E-4736-8D72-117A18AD8279}">
   <dimension ref="B2:E21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1649,282 +1851,282 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="24" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="42">
+      <c r="D3" s="27">
         <v>45751</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="27">
         <v>45752</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="42">
+      <c r="D4" s="27">
         <v>45752</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="27">
         <v>45754</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="42">
+      <c r="D5" s="27">
         <v>45755</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="27">
         <v>45757</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="27">
         <v>45762</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="27">
         <v>45767</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="42">
+      <c r="D7" s="27">
         <v>45766</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="27">
         <v>45767</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="27">
         <v>45768</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="27">
         <v>45768</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="42">
+      <c r="D9" s="27">
         <v>45769</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="27">
         <v>45771</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="42">
+      <c r="D10" s="27">
         <v>45769</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="27">
         <v>45772</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="42">
+      <c r="D11" s="27">
         <v>45773</v>
       </c>
-      <c r="E11" s="42">
+      <c r="E11" s="27">
         <v>45779</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="42">
+      <c r="D12" s="27">
         <v>45780</v>
       </c>
-      <c r="E12" s="42">
+      <c r="E12" s="27">
         <v>45787</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="42">
+      <c r="D13" s="27">
         <v>45788</v>
       </c>
-      <c r="E13" s="42">
+      <c r="E13" s="27">
         <v>45795</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="42">
+      <c r="D14" s="27">
         <v>45788</v>
       </c>
-      <c r="E14" s="42">
+      <c r="E14" s="27">
         <v>45795</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="42">
+      <c r="D15" s="27">
         <v>45796</v>
       </c>
-      <c r="E15" s="42">
+      <c r="E15" s="27">
         <v>45802</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="42">
+      <c r="D16" s="27">
         <v>45803</v>
       </c>
-      <c r="E16" s="42">
+      <c r="E16" s="27">
         <v>45807</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="42">
+      <c r="D17" s="27">
         <v>45808</v>
       </c>
-      <c r="E17" s="42">
+      <c r="E17" s="27">
         <v>45812</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="42">
+      <c r="D18" s="27">
         <v>45813</v>
       </c>
-      <c r="E18" s="42">
+      <c r="E18" s="27">
         <v>45816</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="41" t="s">
+      <c r="C19" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="42">
+      <c r="D19" s="27">
         <v>45817</v>
       </c>
-      <c r="E19" s="42">
+      <c r="E19" s="27">
         <v>45818</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="42">
+      <c r="D20" s="27">
         <v>45819</v>
       </c>
-      <c r="E20" s="42">
+      <c r="E20" s="27">
         <v>45821</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="42">
+      <c r="D21" s="27">
         <v>45822</v>
       </c>
-      <c r="E21" s="42">
+      <c r="E21" s="27">
         <v>45823</v>
       </c>
     </row>
@@ -1938,10 +2140,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0CEC342-310B-4063-9B61-44D1FD29F554}">
-  <dimension ref="B2:F8"/>
+  <dimension ref="B2:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1963,55 +2165,335 @@
       <c r="C3" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="43"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="44" t="s">
-        <v>71</v>
+      <c r="C4" s="29" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="44" t="s">
-        <v>82</v>
+      <c r="C5" s="29" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="44" t="s">
-        <v>83</v>
+      <c r="C6" s="29" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="29" t="s">
         <v>84</v>
-      </c>
-      <c r="C7" s="44" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="44" t="s">
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="45" t="s">
         <v>87</v>
       </c>
+      <c r="C10" s="45"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B14" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="45"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B24" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="45"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B30" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="45"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B38" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42" s="45"/>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" s="29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B46" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B47" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" s="29" t="s">
+        <v>111</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="6">
+    <mergeCell ref="B42:C42"/>
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B34:C34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="6">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cód: Ventana principal V1
</commit_message>
<xml_diff>
--- a/Tablas.xlsx
+++ b/Tablas.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xoel\Desktop\A Carballeira\2DAM\PFC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DEF383-A980-42D9-9846-DADA6CA84947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D020D5-77F4-4973-970C-2A93D1599A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{11D5D283-4BA0-45B7-AEE6-C6A22E61ED0D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{11D5D283-4BA0-45B7-AEE6-C6A22E61ED0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablas BD" sheetId="1" r:id="rId1"/>
     <sheet name="Datos" sheetId="2" r:id="rId2"/>
     <sheet name="Planificación" sheetId="3" r:id="rId3"/>
-    <sheet name="Tablas CU" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="5" r:id="rId4"/>
+    <sheet name="Tablas CU" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="118">
   <si>
     <t>PK</t>
   </si>
@@ -373,6 +374,24 @@
   </si>
   <si>
     <t>Se muestra al usuario un resumen visual o textual de estadísticas como número total de libros, libros leídos, media de calificación, etc.</t>
+  </si>
+  <si>
+    <t>MiBiblio</t>
+  </si>
+  <si>
+    <t>Buscador</t>
+  </si>
+  <si>
+    <t>Filtro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Título libro </t>
+  </si>
+  <si>
+    <t>Portada</t>
+  </si>
+  <si>
+    <t>Icono lupa</t>
   </si>
 </sst>
 </file>
@@ -684,7 +703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -779,18 +798,30 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -800,18 +831,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -819,6 +838,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1439,25 +1461,25 @@
   <sheetData>
     <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="42"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="38"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -1516,24 +1538,24 @@
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="39" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39" t="s">
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1541,29 +1563,29 @@
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="33"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
     </row>
     <row r="6" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="38"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="31"/>
       <c r="E7" s="14"/>
     </row>
@@ -1593,10 +1615,10 @@
       <c r="B10" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="37"/>
+      <c r="D10" s="41"/>
       <c r="E10" s="12"/>
     </row>
     <row r="11" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1677,10 +1699,10 @@
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="35"/>
+      <c r="C24" s="33"/>
     </row>
     <row r="25" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
@@ -1706,10 +1728,10 @@
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="35"/>
+      <c r="C29" s="33"/>
     </row>
     <row r="30" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
@@ -1721,6 +1743,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="G4:G5"/>
@@ -1737,15 +1768,6 @@
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1839,7 +1861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48A83546-915E-4736-8D72-117A18AD8279}">
   <dimension ref="B2:E21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -2139,6 +2161,52 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B13A910-58EA-4D73-9420-5D74A603EB17}">
+  <dimension ref="B2:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="46"/>
+      <c r="D4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:C4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0CEC342-310B-4063-9B61-44D1FD29F554}">
   <dimension ref="B2:F48"/>
   <sheetViews>

</xml_diff>

<commit_message>
Dóc: Correción casos de uso. Estudio de mercado. Presupuesto. Webgrafía
</commit_message>
<xml_diff>
--- a/Tablas.xlsx
+++ b/Tablas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xoel\Desktop\A Carballeira\2DAM\PFC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D020D5-77F4-4973-970C-2A93D1599A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DD982F-82F6-43B7-A2E8-9CC747FCE346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{11D5D283-4BA0-45B7-AEE6-C6A22E61ED0D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{11D5D283-4BA0-45B7-AEE6-C6A22E61ED0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablas BD" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="133">
   <si>
     <t>PK</t>
   </si>
@@ -271,9 +271,6 @@
     <t>Ver estadísticas (número de libros leídos, promedio de calificación, etc.)</t>
   </si>
   <si>
-    <t>CASO DE USO 1: AÑADIR UN LIBRO</t>
-  </si>
-  <si>
     <t>Campo</t>
   </si>
   <si>
@@ -286,9 +283,6 @@
     <t>Actor</t>
   </si>
   <si>
-    <t>El usuario pulsa el botón "+" para añadir un libro. Introduce el título, autor o ISBN en el buscador y se muestran las posibles coincidencias. Al seleccionar un libro, este se añade a su biblioteca personal con los datos recuperados automáticamente desde la API (si están disponibles).</t>
-  </si>
-  <si>
     <t>Precondición</t>
   </si>
   <si>
@@ -301,9 +295,6 @@
     <t>El libro queda registrado en la biblioteca del usuario. A nivel interno, si el autor, género o editorial no existiera previamente en la base de datos, se crean automáticamente para mantener las relaciones correctas.</t>
   </si>
   <si>
-    <t>CASO DE USO 2: EDITAR UN LIBRO</t>
-  </si>
-  <si>
     <t>El usuario accede a los detalles de un libro previamente añadido y modifica uno o varios campos: fechas de lectura, reseña personal, calificación, estado, etc.</t>
   </si>
   <si>
@@ -313,69 +304,15 @@
     <t>El libro ya debe estar registrado en la biblioteca del usuario.</t>
   </si>
   <si>
-    <t>Añadir un libro.</t>
-  </si>
-  <si>
     <t>Usuario.</t>
   </si>
   <si>
-    <t>Editar un libro.</t>
-  </si>
-  <si>
-    <t>CASO DE USO 3: ELIMINAR UN LIBRO</t>
-  </si>
-  <si>
-    <t>Eliminar un libro.</t>
-  </si>
-  <si>
     <t>El usuario selecciona un libro de su biblioteca personal y lo elimina permanentemente.</t>
   </si>
   <si>
     <t>El libro se elimina de la base de datos. Las relaciones con autores, géneros o editorial también se eliminan si ya no están vinculadas a otros libros.</t>
   </si>
   <si>
-    <t>CASO DE USO 4: BUSCAR LIBROS</t>
-  </si>
-  <si>
-    <t>Buscar libros.</t>
-  </si>
-  <si>
-    <t>Desde la vista principal (vista en la que se muestran los libros añadidos por el usuario a su biblioteca), el usuario introduce un término de búsqueda (título, autor o ISBN) en el buscador para localizar libros específicos.</t>
-  </si>
-  <si>
-    <t>Deben existir libros previamente añadidos por el usuario.</t>
-  </si>
-  <si>
-    <t>La vista principal se actualiza mostrando únicamente los libros que coinciden con el criterio de búsqueda.</t>
-  </si>
-  <si>
-    <t>CASO DE USO 5: FILTRAR LIBROS</t>
-  </si>
-  <si>
-    <t>Filtrar libros.</t>
-  </si>
-  <si>
-    <t>El usuario aplica uno o varios filtros desde la interfaz principal para visualizar solo los libros que cumplan ciertos criterios: género, serie, estado, calificación, etc.</t>
-  </si>
-  <si>
-    <t>La lista de libros mostrada se actualiza para reflejar solo aquellos que cumplen con los filtros aplicados.</t>
-  </si>
-  <si>
-    <t>CASO DE USO 6: VER ESTADÍSTICAS</t>
-  </si>
-  <si>
-    <t>Ver estadísticas.</t>
-  </si>
-  <si>
-    <t>El usuario accede a una sección de la aplicación que muestra datos estadísticos basados en los libros de su biblioteca.</t>
-  </si>
-  <si>
-    <t>Deben existir libros añadidos con información suficiente (estado de lectura, calificación, fechas, etc.).</t>
-  </si>
-  <si>
-    <t>Se muestra al usuario un resumen visual o textual de estadísticas como número total de libros, libros leídos, media de calificación, etc.</t>
-  </si>
-  <si>
     <t>MiBiblio</t>
   </si>
   <si>
@@ -392,13 +329,875 @@
   </si>
   <si>
     <t>Icono lupa</t>
+  </si>
+  <si>
+    <t>Crear un libro.</t>
+  </si>
+  <si>
+    <t>CASO DE USO 1: INICIAR APLICACIÓN</t>
+  </si>
+  <si>
+    <t>Al arrancar la aplicación, se crea la base de datos si no existe, y se muestra la ventana principal con el listado de libros guardados (en el caso de haberlos).</t>
+  </si>
+  <si>
+    <t>Ninguna.</t>
+  </si>
+  <si>
+    <t>Flujo principal</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ejecución script principal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se crea o se abre la base de datos </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se instancian los componentes de la ventana principal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se consultan las diferente tablas de la base de datos para obtener el listado </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se muestran los libros (de haberlos) o un mensaje "No hay libros guardados" (de no haberlos)</t>
+    </r>
+  </si>
+  <si>
+    <t>Se muestra la ventana principal.</t>
+  </si>
+  <si>
+    <t>Se muestran todos los libros guardados en la base de datos, con su título, autor, año, estado y portada.</t>
+  </si>
+  <si>
+    <t>La ventana principal está iniciada y la base de datos creada.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Se obtienen los libros guardados en la base de datos </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→ Se itera sobre cada libro</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Para cada libro se determina el color de fondo según su estado y se crea un frame con el título, el autor, el año y la portada </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se muestran todos los frames</t>
+    </r>
+  </si>
+  <si>
+    <t>Si no hay libros se muestra: "No hay libros guardados". Si falla la carga de portada, se usa una imagen predeterminada "Sin portada".</t>
+  </si>
+  <si>
+    <t>Se muestra la lista en pantalla y el usuario puede interactuar.</t>
+  </si>
+  <si>
+    <t>CASO DE USO 2: VER LISTADO DE LIBROS</t>
+  </si>
+  <si>
+    <t>CASO DE USO 3: BUSCAR LIBROS GUARDADOS</t>
+  </si>
+  <si>
+    <t>Se realiza una búsqueda de los libros guardados por título o autor.</t>
+  </si>
+  <si>
+    <t>Ventana principal abierta y listado inicial cargado.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">El usuario introduce texto en el campo de búsqueda y pulsa el botón de buscar </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→ La app recoje el texto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se ejecuta sentencia SQL para hacer búsqueda por título o autor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Si hay resultados se muestran los libros filtrados, si no se muestra: "No se encontraron libros que coincidan" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Si el buscador está vacío y se pulsa el botón de búsqueda se recarga el listado completo</t>
+    </r>
+  </si>
+  <si>
+    <t>Error en la consulta: mostrar messagebox de error.</t>
+  </si>
+  <si>
+    <t>Vista refrescada con los libros filtrados o con todos si la búsqueda está vacía.</t>
+  </si>
+  <si>
+    <t>CASO DE USO 4: AÑADIR UN LIBRO</t>
+  </si>
+  <si>
+    <t>El usuario busca un libro por título, autor o ISBN, se muestran los resultados y se guarda el libro seleccionado en la base de datos.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">El usuario pulsa el botón "+" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se abre una ventana de elección (Crear o Añadir) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Selecciona "Añadir libro" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se abre la ventana de añadir libro </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> El usuario escribe el texto de búsqueda y pulsa buscar </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se hace una llamada a la API de OpenLibrary y se extraen los datos de búsqueda correspondientes </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se muestra cada resultado en una tarjeta con título, autor, año y portada (si los datos existen) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> El usuario selecciona un libro cuyos datos se insertan en la BD </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se muestra: "Libro guardado correctamente" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se recarga el listado de la ventana principal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> El usuario cierra la ventana de búsqueda o sigue buscando</t>
+    </r>
+  </si>
+  <si>
+    <t>Flujos alternativos</t>
+  </si>
+  <si>
+    <t>Si el libro ya existe (ISBN duplicado) se ignora. El usuario puede cancelar sin seleccionar un libro.</t>
+  </si>
+  <si>
+    <t>CASO DE USO 5: CREAR UN LIBRO</t>
+  </si>
+  <si>
+    <t>Permite al  usuario crear un libro manualmente (todos los campos editables) cuando la búsqueda no arroja los resultados deseados.</t>
+  </si>
+  <si>
+    <t>Ventana principal abierta.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">El usuario pulsa el botón "+" y elige "Crear libro" en la ventana de elección </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se abre la ventana de editar libro con todos los campos del formulario vacíos </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> El usuario rellena los campos que crea convenientes y puede insertar una imagen en la portada </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> El usuario guarda los cambios </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se muestra: "Libro creado correctamente" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se recarga el listado principal</t>
+    </r>
+  </si>
+  <si>
+    <t>Error al insertar: se muestra el error. El usuario puede pulsar "Cancelar": la ventana se cierra sin guardar nada.</t>
+  </si>
+  <si>
+    <t>Si guardó, aparece en el listado principal.</t>
+  </si>
+  <si>
+    <t>CASO DE USO 6: EDITAR UN LIBRO</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">El usuario selecciona un libro del listado principal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se abre la ventana de edición </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se cargan los datos del libro </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> El usuario modifica uno o varios campos </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> El usuario guarda los cambios </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se muestra: "Libro actualizado correctamente" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se cierra la ventan y se recarga el listado principal</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Error en la BD: se muestra el error. El usuario pulsa "Eliminar libro" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se solicita confirmación </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se eliminan datos y relaciones </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se muestra: "Libro eliminado" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se cierra la ventana y se recarga el listado principal. El usuario pulsa "Cancelar": descarta cambios y cierra la ventana.</t>
+    </r>
+  </si>
+  <si>
+    <t>CASO DE USO 7: ELIMINAR UN LIBRO</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">El usuario selecciona un libro del listado principal → Se abre la ventana de edición → Se cargan los datos del libro → El usuario pulsa "Eliminar libro" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Aparece diálogo de confirmación </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Si confirma se eliminan los datos y relaciones del libro </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se muestra: "Libro eliminado correctamente" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Se cierra la ventana y se recarga el listado principal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Si el usuario cancela, se cierra el diálogo y no hace nada</t>
+    </r>
+  </si>
+  <si>
+    <t>Error durante la eliminación: mostrar error.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,6 +1231,18 @@
       <sz val="10.5"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -703,7 +1514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -792,24 +1603,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -819,35 +1642,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="28">
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -897,6 +1711,21 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1034,7 +1863,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3580BE9-19D9-4226-A531-EAB7E1E7B707}" name="Tabla1" displayName="Tabla1" ref="B2:E21" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3580BE9-19D9-4226-A531-EAB7E1E7B707}" name="Tabla1" displayName="Tabla1" ref="B2:E21" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="B2:E21" xr:uid="{A3580BE9-19D9-4226-A531-EAB7E1E7B707}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1042,94 +1871,108 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{02BCE4A8-9E29-4081-86C4-CC2E1D82791E}" name="Fase" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{C8D57AC5-20ED-437C-8900-3789D4A8BC25}" name="Tiempo estimado" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{DAE254B1-C70D-458D-973F-5006E8EBEB8B}" name="Inicio" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{C0EA90E3-1365-4B0A-805E-83353688EC11}" name="Fin" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{02BCE4A8-9E29-4081-86C4-CC2E1D82791E}" name="Fase" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{C8D57AC5-20ED-437C-8900-3789D4A8BC25}" name="Tiempo estimado" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{DAE254B1-C70D-458D-973F-5006E8EBEB8B}" name="Inicio" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{C0EA90E3-1365-4B0A-805E-83353688EC11}" name="Fin" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{35D9FBFC-1314-4A7C-A358-B29E72364FB8}" name="Tabla5" displayName="Tabla5" ref="B3:C8" totalsRowShown="0" headerRowDxfId="17">
-  <autoFilter ref="B3:C8" xr:uid="{35D9FBFC-1314-4A7C-A358-B29E72364FB8}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{35D9FBFC-1314-4A7C-A358-B29E72364FB8}" name="Tabla5" displayName="Tabla5" ref="B29:C35" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="B29:C35" xr:uid="{35D9FBFC-1314-4A7C-A358-B29E72364FB8}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{B9465E2E-C568-499E-BA0C-90A7552A7662}" name="Campo" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{3CF3611C-CFF7-4246-930B-F666D8CA7927}" name="Descripción" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{B9465E2E-C568-499E-BA0C-90A7552A7662}" name="Campo" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{3CF3611C-CFF7-4246-930B-F666D8CA7927}" name="Descripción" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4AAE1917-C13A-4CDF-B275-F08A045DAFE6}" name="Tabla53" displayName="Tabla53" ref="B11:C16" totalsRowShown="0" headerRowDxfId="14">
-  <autoFilter ref="B11:C16" xr:uid="{4AAE1917-C13A-4CDF-B275-F08A045DAFE6}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4AAE1917-C13A-4CDF-B275-F08A045DAFE6}" name="Tabla53" displayName="Tabla53" ref="B48:C54" totalsRowShown="0" headerRowDxfId="18">
+  <autoFilter ref="B48:C54" xr:uid="{4AAE1917-C13A-4CDF-B275-F08A045DAFE6}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{746F11CB-73EF-48D0-A103-6082BFA4840D}" name="Campo" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{5A63AE89-EBA0-4B1C-A759-57B1454AD949}" name="Descripción" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{746F11CB-73EF-48D0-A103-6082BFA4840D}" name="Campo" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{5A63AE89-EBA0-4B1C-A759-57B1454AD949}" name="Descripción" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C92D463C-1773-45B1-BE84-D28B2B4C0FD3}" name="Tabla534" displayName="Tabla534" ref="B19:C24" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="B19:C24" xr:uid="{C92D463C-1773-45B1-BE84-D28B2B4C0FD3}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C92D463C-1773-45B1-BE84-D28B2B4C0FD3}" name="Tabla534" displayName="Tabla534" ref="B57:C63" totalsRowShown="0" headerRowDxfId="15">
+  <autoFilter ref="B57:C63" xr:uid="{C92D463C-1773-45B1-BE84-D28B2B4C0FD3}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{B0231060-EB1A-414C-9CB7-2B3555D1B5EB}" name="Campo" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{283AE2CC-2976-4B96-9CBB-8DA22B7E4BBC}" name="Descripción" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{B0231060-EB1A-414C-9CB7-2B3555D1B5EB}" name="Campo" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{283AE2CC-2976-4B96-9CBB-8DA22B7E4BBC}" name="Descripción" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{28243E43-C480-424E-AE9B-4642FA5901BA}" name="Tabla5345" displayName="Tabla5345" ref="B27:C32" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="B27:C32" xr:uid="{28243E43-C480-424E-AE9B-4642FA5901BA}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{CB2D3D08-BAD0-45B7-8F5B-2E2AEA7ED75A}" name="Tabla511" displayName="Tabla511" ref="B38:C45" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="B38:C45" xr:uid="{CB2D3D08-BAD0-45B7-8F5B-2E2AEA7ED75A}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{495E8330-EB37-43CF-AD89-2059C11F972B}" name="Campo" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{E698F615-40DE-4255-8FE4-E9BE3ED6621B}" name="Descripción" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{1931B87D-7BEC-48F6-91E1-059BD8C163D1}" name="Campo" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{E59DDA27-C0AF-4A90-92EF-8D23C7CEA319}" name="Descripción" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BBED26D4-7CB2-43A3-8A0D-EFB57C8CBCAE}" name="Tabla53457" displayName="Tabla53457" ref="B35:C40" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="B35:C40" xr:uid="{BBED26D4-7CB2-43A3-8A0D-EFB57C8CBCAE}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6A69E14E-D88E-471F-BA05-0E1DEB350E33}" name="Tabla512" displayName="Tabla512" ref="B3:C8" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="B3:C8" xr:uid="{6A69E14E-D88E-471F-BA05-0E1DEB350E33}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{7B66B3BD-5CF1-4705-9F4D-0354B9C0BF7A}" name="Campo" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{2EA9C0F4-971D-400D-93DB-A3567A1FAF38}" name="Descripción" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{89167888-21FF-4C1A-9273-8A20BA27D9B1}" name="Campo" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{AF80A923-A0BA-43FF-9A4A-AD6E594093FC}" name="Descripción" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1B74E673-8337-4E9D-AC1A-1CD7434921E6}" name="Tabla534578" displayName="Tabla534578" ref="B43:C48" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="B43:C48" xr:uid="{1B74E673-8337-4E9D-AC1A-1CD7434921E6}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4CF03345-C244-41E6-AD8F-44B49070C82B}" name="Tabla51213" displayName="Tabla51213" ref="B11:C17" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="B11:C17" xr:uid="{4CF03345-C244-41E6-AD8F-44B49070C82B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3F70A758-7B26-45A9-AA70-7C6ECE322353}" name="Campo" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{AFB2C923-0B4F-4BE0-ABBA-BD129C347F42}" name="Descripción" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{0A18BCF9-BD3B-4A39-98A1-121FDFF8884A}" name="Campo" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{6AEDE57B-E6D8-4173-9CEA-58401435415E}" name="Descripción" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{6A48FFE3-02CA-44AE-9413-616609B5EBFD}" name="Tabla5121314" displayName="Tabla5121314" ref="B20:C26" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="B20:C26" xr:uid="{6A48FFE3-02CA-44AE-9413-616609B5EBFD}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{ED47321F-6D62-4426-B264-CB565C2AD64C}" name="Campo" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{660C5A4E-2650-4941-9D7F-80B752A88435}" name="Descripción" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1461,25 +2304,25 @@
   <sheetData>
     <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="38"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="42"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -1538,24 +2381,24 @@
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="34" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="34"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="34" t="s">
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1563,30 +2406,30 @@
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
     </row>
     <row r="6" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="31"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="38"/>
       <c r="E7" s="14"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
@@ -1615,18 +2458,18 @@
       <c r="B10" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="41"/>
+      <c r="D10" s="35"/>
       <c r="E10" s="12"/>
     </row>
     <row r="11" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="31"/>
+      <c r="C12" s="38"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
@@ -1654,10 +2497,10 @@
     </row>
     <row r="16" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="31"/>
+      <c r="C17" s="38"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
@@ -1685,10 +2528,10 @@
     </row>
     <row r="21" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="31"/>
+      <c r="C22" s="38"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
@@ -1714,10 +2557,10 @@
     </row>
     <row r="26" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="31"/>
+      <c r="C27" s="38"/>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="9" t="s">
@@ -1743,15 +2586,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="G4:G5"/>
@@ -1768,6 +2602,15 @@
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="B17:C17"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2164,7 +3007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B13A910-58EA-4D73-9420-5D74A603EB17}">
   <dimension ref="B2:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -2172,29 +3015,29 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
+      <c r="B3" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="46" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4" s="46"/>
+      <c r="B4" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="45"/>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2208,360 +3051,480 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0CEC342-310B-4063-9B61-44D1FD29F554}">
-  <dimension ref="B2:F48"/>
+  <dimension ref="B2:F63"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="45" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="46"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="45"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" s="28"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>80</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="29" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
-        <v>79</v>
-      </c>
       <c r="C6" s="29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="75" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="29" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
-        <v>85</v>
-      </c>
       <c r="C8" s="29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="45"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="46"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>80</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="29" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
-        <v>79</v>
-      </c>
       <c r="C14" s="29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="46"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="29" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="14" t="s">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="B24" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="29" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C16" s="29" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="45" t="s">
-        <v>94</v>
-      </c>
-      <c r="C18" s="45"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
+      <c r="C26" s="29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" s="46"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="14" t="s">
+      <c r="F29" s="28"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="29" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="14" t="s">
+      <c r="C30" s="29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="29" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="14" t="s">
+      <c r="C32" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="B33" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B34" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" s="47" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B35" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="29" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B24" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="C26" s="45"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="12" t="s">
+      <c r="C35" s="29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="14"/>
+      <c r="C36" s="29"/>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" s="46"/>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" s="29" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B30" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C30" s="29" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B32" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="C34" s="45"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="29" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" s="29" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B38" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" s="29" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="14" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C39" s="29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" s="29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B41" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B43" s="14" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B40" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C40" s="29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="45" t="s">
-        <v>107</v>
-      </c>
-      <c r="C42" s="45"/>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B44" s="14" t="s">
-        <v>80</v>
+        <v>119</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="14"/>
+      <c r="C46" s="29"/>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="C47" s="46"/>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B50" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50" s="29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C45" s="29" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B46" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C46" s="29" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B47" s="14" t="s">
+      <c r="C51" s="29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B52" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" s="29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B53" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C53" s="29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B54" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C47" s="29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C48" s="29" t="s">
-        <v>111</v>
+      <c r="C54" s="29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="C56" s="46"/>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C58" s="29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B59" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C59" s="29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C60" s="29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="B61" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C61" s="29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62" s="29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B63" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C63" s="29" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B42:C42"/>
+  <mergeCells count="7">
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B37:C37"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B19:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="6">
+  <tableParts count="7">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>